<commit_message>
add w5 video link
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule_updated.xlsx
+++ b/docs/nopublish/schedule_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDEBE0D-DA00-4289-B31E-BDA91D5CD07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0138CB05-3C76-4844-8E7C-B5EF79205590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="273">
   <si>
     <t>Week</t>
   </si>
@@ -846,6 +846,12 @@
   </si>
   <si>
     <t>hw5.html</t>
+  </si>
+  <si>
+    <t>https://uoregon.zoom.us/rec/share/NC_wGI1uK50qx4h99kyrGdzw1FaXAwjatpj6T_sYv8H_inyAPOuBvsQvJwYyWh8v.RRQOUwFiWqf8app0</t>
+  </si>
+  <si>
+    <t>e4^QAsi?</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1482,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1835,30 +1841,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
-    <col min="11" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" customWidth="1"/>
+    <col min="11" max="13" width="16.86328125" customWidth="1"/>
+    <col min="14" max="14" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.42578125" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.3984375" customWidth="1"/>
+    <col min="20" max="20" width="56.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="23" customFormat="1">
@@ -2025,7 +2031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" s="8" customFormat="1" ht="14.65" thickBot="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2581,6 +2587,12 @@
       </c>
       <c r="K21" s="11" t="s">
         <v>119</v>
+      </c>
+      <c r="L21" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="N21" s="11" t="s">
         <v>124</v>
@@ -3158,9 +3170,10 @@
     <hyperlink ref="P25" r:id="rId11" xr:uid="{63E34C6F-6ADA-4E7B-9F9A-C4BA22381F5C}"/>
     <hyperlink ref="S30" r:id="rId12" xr:uid="{50853C36-94D7-493B-AC3E-9B4E913FC0D7}"/>
     <hyperlink ref="P26" r:id="rId13" xr:uid="{24954DE6-A619-4130-94FF-153270EF287A}"/>
+    <hyperlink ref="L21" r:id="rId14" xr:uid="{687C1A49-5786-4E3B-84FF-19F5297AC4AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -3172,11 +3185,11 @@
       <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4077,21 +4090,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.86328125" customWidth="1"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1"/>
+    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4256,7 +4269,7 @@
       <c r="E6" t="s">
         <v>220</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" t="s">
         <v>270</v>
       </c>
       <c r="H6">

</xml_diff>

<commit_message>
update assignments & sched for w7
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule_updated.xlsx
+++ b/docs/nopublish/schedule_updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D11DCE4-7C99-4652-9A22-1EE9DB60EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD4E1A4-2325-4155-9B87-780B331B3217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="280">
   <si>
     <t>Week</t>
   </si>
@@ -864,6 +864,15 @@
   </si>
   <si>
     <t>7Rm!W?tm</t>
+  </si>
+  <si>
+    <t>hw8.html</t>
+  </si>
+  <si>
+    <t>hw5-key.Rmd</t>
+  </si>
+  <si>
+    <t>hw7.Rmd</t>
   </si>
 </sst>
 </file>
@@ -1853,9 +1862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="O1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2863,7 +2872,9 @@
       <c r="O29" t="s">
         <v>145</v>
       </c>
-      <c r="P29" s="27"/>
+      <c r="P29" s="27" t="s">
+        <v>277</v>
+      </c>
       <c r="Q29" s="11" t="s">
         <v>98</v>
       </c>
@@ -2974,7 +2985,9 @@
       <c r="R33" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="S33" s="27"/>
+      <c r="S33" s="27" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="34" spans="1:24" s="2" customFormat="1">
       <c r="A34" s="2">
@@ -4112,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4302,6 +4315,9 @@
       <c r="I6" t="s">
         <v>230</v>
       </c>
+      <c r="J6" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
@@ -4353,6 +4369,9 @@
       <c r="I8" t="s">
         <v>215</v>
       </c>
+      <c r="J8" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
@@ -4370,7 +4389,9 @@
       <c r="E9" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" t="s">
+        <v>277</v>
+      </c>
       <c r="H9">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
update main pages with hws
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule_updated.xlsx
+++ b/docs/nopublish/schedule_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1741C5-45B3-4277-80BD-13196DD76EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEAB6DC-637A-40F2-B7C3-4D372F385902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="283">
   <si>
     <t>Week</t>
   </si>
@@ -879,6 +879,9 @@
   </si>
   <si>
     <t>^4r!dSVA</t>
+  </si>
+  <si>
+    <t>hw9.html</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1460,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1510,6 +1513,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1868,9 +1872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomLeft" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2988,7 +2992,9 @@
       <c r="O33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="P33" s="29"/>
+      <c r="P33" s="29" t="s">
+        <v>282</v>
+      </c>
       <c r="Q33" s="1" t="s">
         <v>223</v>
       </c>
@@ -3102,7 +3108,9 @@
       <c r="R37" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="S37" s="30"/>
+      <c r="S37" s="30" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="38" spans="1:24" s="8" customFormat="1">
       <c r="A38" s="8">
@@ -4136,7 +4144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -4427,7 +4435,9 @@
       <c r="E10" t="s">
         <v>224</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="38" t="s">
+        <v>282</v>
+      </c>
       <c r="H10">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
add hw keys 9 & 10
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule_updated.xlsx
+++ b/docs/nopublish/schedule_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA74059-374C-4970-A538-2200BE105437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133686E0-A284-43BA-92FE-3DA1DA26CD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="291">
   <si>
     <t>Week</t>
   </si>
@@ -900,6 +900,12 @@
   </si>
   <si>
     <t>9.^4GaF&amp;</t>
+  </si>
+  <si>
+    <t>hw9-key.Rmd</t>
+  </si>
+  <si>
+    <t>hw10.Rmd</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1490,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1538,7 +1544,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="42" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1897,30 +1902,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L38" sqref="L38"/>
+    <sheetView topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.86328125" customWidth="1"/>
-    <col min="5" max="5" width="19.3984375" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="31.59765625" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.73046875" customWidth="1"/>
-    <col min="11" max="13" width="16.86328125" customWidth="1"/>
-    <col min="14" max="14" width="47.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="11" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="36.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.3984375" customWidth="1"/>
-    <col min="20" max="20" width="56.73046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.42578125" customWidth="1"/>
+    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="23" customFormat="1">
@@ -1985,7 +1990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15">
+    <row r="2" spans="1:20" ht="15.75">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2087,7 +2092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="8" customFormat="1" ht="14.65" thickBot="1">
+    <row r="5" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2106,7 +2111,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="15">
+    <row r="6" spans="1:20" s="2" customFormat="1" ht="15.75">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2458,7 +2463,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" ht="15">
+    <row r="16" spans="1:20" s="2" customFormat="1" ht="15.75">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="1" customFormat="1" ht="15">
+    <row r="25" spans="1:20" s="1" customFormat="1" ht="15.75">
       <c r="A25" s="1">
         <v>6</v>
       </c>
@@ -3128,7 +3133,7 @@
       <c r="L37" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="M37" s="39" t="s">
+      <c r="M37" t="s">
         <v>288</v>
       </c>
       <c r="N37" s="11" t="s">
@@ -3188,7 +3193,9 @@
       <c r="R39" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="S39" s="27"/>
+      <c r="S39" s="30" t="s">
+        <v>286</v>
+      </c>
       <c r="T39" s="2" t="s">
         <v>174</v>
       </c>
@@ -3279,11 +3286,11 @@
       <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4184,21 +4191,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="47.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.86328125" customWidth="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1"/>
-    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4486,7 +4493,9 @@
       <c r="I10" t="s">
         <v>233</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
@@ -4513,7 +4522,9 @@
       <c r="I11" t="s">
         <v>234</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">

</xml_diff>